<commit_message>
Commit some models (app probably not running now)
</commit_message>
<xml_diff>
--- a/my_codebook.xlsx
+++ b/my_codebook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julia/Desktop/Gov 1005/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F97C98-76E4-1D44-9E32-C45AF2DD9796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5909B0-62C3-2C4F-82E5-6129C78FFB98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14940" windowHeight="16120" xr2:uid="{D8828246-9BF0-C24B-93D3-DBEE112670D2}"/>
+    <workbookView xWindow="13860" yWindow="460" windowWidth="14940" windowHeight="16120" xr2:uid="{D8828246-9BF0-C24B-93D3-DBEE112670D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -932,7 +932,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Commit all shiny components
</commit_message>
<xml_diff>
--- a/my_codebook.xlsx
+++ b/my_codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julia/Desktop/Gov 1005/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5909B0-62C3-2C4F-82E5-6129C78FFB98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8664BBE9-47EE-E745-AFC6-FC133E70D71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13860" yWindow="460" windowWidth="14940" windowHeight="16120" xr2:uid="{D8828246-9BF0-C24B-93D3-DBEE112670D2}"/>
   </bookViews>
@@ -932,7 +932,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Final commit of ms_8 draft (sans original datafiles)
</commit_message>
<xml_diff>
--- a/my_codebook.xlsx
+++ b/my_codebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julia/Desktop/Gov 1005/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8664BBE9-47EE-E745-AFC6-FC133E70D71D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48E3DCA-8A80-5649-BADF-8209D59B67A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="460" windowWidth="14940" windowHeight="16120" xr2:uid="{D8828246-9BF0-C24B-93D3-DBEE112670D2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15040" windowHeight="15940" xr2:uid="{D8828246-9BF0-C24B-93D3-DBEE112670D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>female</t>
   </si>
   <si>
-    <t xml:space="preserve">total population attending school </t>
-  </si>
-  <si>
     <t>school male</t>
   </si>
   <si>
@@ -546,6 +543,9 @@
   </si>
   <si>
     <t>B2J001/B18001*101</t>
+  </si>
+  <si>
+    <t>enrolled</t>
   </si>
 </sst>
 </file>
@@ -932,7 +932,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -979,31 +979,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1011,51 +1011,51 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1063,42 +1063,42 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1108,16 +1108,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1125,31 +1125,31 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1157,63 +1157,63 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" t="s">
-        <v>67</v>
-      </c>
       <c r="F11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1221,31 +1221,31 @@
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1253,69 +1253,69 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1327,14 +1327,14 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1346,70 +1346,70 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" t="s">
         <v>96</v>
       </c>
-      <c r="D19" t="s">
-        <v>97</v>
-      </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" t="s">
         <v>135</v>
       </c>
-      <c r="H19" t="s">
-        <v>136</v>
-      </c>
       <c r="J19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1422,183 +1422,183 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" t="s">
         <v>52</v>
       </c>
-      <c r="D23" t="s">
-        <v>53</v>
-      </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" t="s">
         <v>93</v>
       </c>
-      <c r="E24" t="s">
-        <v>94</v>
-      </c>
       <c r="F24" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" t="s">
         <v>110</v>
       </c>
-      <c r="G24" t="s">
-        <v>111</v>
-      </c>
       <c r="H24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="C26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="D27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="E28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="F29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="G30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I33" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="I34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="I35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:11">
       <c r="J36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="J37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="J38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="K39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="K40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>